<commit_message>
alteracoes nos meses (ingles)
</commit_message>
<xml_diff>
--- a/DEC-FEC Polos.xlsx
+++ b/DEC-FEC Polos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jcruzpir_emeal_nttdata_com/Documents/Escritorio/PEM_NPEM DEC-FEC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{B0EEC49E-532A-490F-B091-DC302BCD891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="6_{B0EEC49E-532A-490F-B091-DC302BCD891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBFDF9E5-E9C0-42D4-A068-7A553E338DD8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Campos</t>
   </si>
@@ -136,6 +136,39 @@
   </si>
   <si>
     <t>ago/24</t>
+  </si>
+  <si>
+    <t>feb/23</t>
+  </si>
+  <si>
+    <t>apr/23</t>
+  </si>
+  <si>
+    <t>may/23</t>
+  </si>
+  <si>
+    <t>aug/23</t>
+  </si>
+  <si>
+    <t>sep/23</t>
+  </si>
+  <si>
+    <t>oct/23</t>
+  </si>
+  <si>
+    <t>dec/23</t>
+  </si>
+  <si>
+    <t>feb/24</t>
+  </si>
+  <si>
+    <t>apr/24</t>
+  </si>
+  <si>
+    <t>may/24</t>
+  </si>
+  <si>
+    <t>aug/24</t>
   </si>
 </sst>
 </file>
@@ -463,7 +496,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E9" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,7 +585,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>0.39557110367033427</v>
@@ -634,7 +667,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>0.58969043256189624</v>
@@ -675,7 +708,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>0.55398246208563939</v>
@@ -798,7 +831,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>0.51954951669294391</v>
@@ -839,7 +872,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>0.70470077285349764</v>
@@ -880,7 +913,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>0.40089830024750733</v>
@@ -962,7 +995,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>0.60154821343246789</v>
@@ -1044,7 +1077,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>0.41176264633640508</v>
@@ -1126,7 +1159,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0.70365445706562779</v>
@@ -1167,7 +1200,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0.66666755683012968</v>
@@ -1290,7 +1323,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>0.9</v>

</xml_diff>

<commit_message>
alteracao no locale para pt (meses para pt tbm)
</commit_message>
<xml_diff>
--- a/DEC-FEC Polos.xlsx
+++ b/DEC-FEC Polos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jcruzpir_emeal_nttdata_com/Documents/Escritorio/PEM_NPEM DEC-FEC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="6_{B0EEC49E-532A-490F-B091-DC302BCD891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{848E2984-2DF7-4F9D-8025-206E0D3B6BBD}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="6_{B0EEC49E-532A-490F-B091-DC302BCD891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A347DA0B-7291-4CF6-A2AC-B74531552B82}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEC" sheetId="1" r:id="rId1"/>
@@ -105,40 +105,40 @@
     <t>jul/24</t>
   </si>
   <si>
-    <t>feb/23</t>
-  </si>
-  <si>
-    <t>apr/23</t>
-  </si>
-  <si>
-    <t>may/23</t>
-  </si>
-  <si>
-    <t>aug/23</t>
-  </si>
-  <si>
-    <t>sep/23</t>
-  </si>
-  <si>
-    <t>oct/23</t>
-  </si>
-  <si>
-    <t>dec/23</t>
-  </si>
-  <si>
-    <t>feb/24</t>
-  </si>
-  <si>
-    <t>apr/24</t>
-  </si>
-  <si>
-    <t>may/24</t>
-  </si>
-  <si>
-    <t>aug/24</t>
-  </si>
-  <si>
-    <t>sep/24</t>
+    <t>fev/23</t>
+  </si>
+  <si>
+    <t>abr/23</t>
+  </si>
+  <si>
+    <t>mai/23</t>
+  </si>
+  <si>
+    <t>ago/23</t>
+  </si>
+  <si>
+    <t>set/23</t>
+  </si>
+  <si>
+    <t>out/23</t>
+  </si>
+  <si>
+    <t>dez/23</t>
+  </si>
+  <si>
+    <t>fev/24</t>
+  </si>
+  <si>
+    <t>abr/24</t>
+  </si>
+  <si>
+    <t>mai/24</t>
+  </si>
+  <si>
+    <t>ago/24</t>
+  </si>
+  <si>
+    <t>set/24</t>
   </si>
 </sst>
 </file>
@@ -180,9 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1372,6 +1373,9 @@
       <c r="M22">
         <v>0.65</v>
       </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1386,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C8BAD7-93A4-4488-8240-EF1411275326}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
alteracoes nos meses para ingles
</commit_message>
<xml_diff>
--- a/DEC-FEC Polos.xlsx
+++ b/DEC-FEC Polos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/jcruzpir_emeal_nttdata_com/Documents/Escritorio/PEM_NPEM DEC-FEC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="6_{B0EEC49E-532A-490F-B091-DC302BCD891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A347DA0B-7291-4CF6-A2AC-B74531552B82}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="6_{B0EEC49E-532A-490F-B091-DC302BCD891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76DB5AE9-D51B-4CC3-A951-6805E0191403}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEC" sheetId="1" r:id="rId1"/>
@@ -105,40 +105,40 @@
     <t>jul/24</t>
   </si>
   <si>
-    <t>fev/23</t>
-  </si>
-  <si>
-    <t>abr/23</t>
-  </si>
-  <si>
-    <t>mai/23</t>
-  </si>
-  <si>
-    <t>ago/23</t>
-  </si>
-  <si>
-    <t>set/23</t>
-  </si>
-  <si>
-    <t>out/23</t>
-  </si>
-  <si>
-    <t>dez/23</t>
-  </si>
-  <si>
-    <t>fev/24</t>
-  </si>
-  <si>
-    <t>abr/24</t>
-  </si>
-  <si>
-    <t>mai/24</t>
-  </si>
-  <si>
-    <t>ago/24</t>
-  </si>
-  <si>
-    <t>set/24</t>
+    <t>feb/23</t>
+  </si>
+  <si>
+    <t>apr/23</t>
+  </si>
+  <si>
+    <t>may/23</t>
+  </si>
+  <si>
+    <t>aug/23</t>
+  </si>
+  <si>
+    <t>sep/23</t>
+  </si>
+  <si>
+    <t>oct/23</t>
+  </si>
+  <si>
+    <t>dec/23</t>
+  </si>
+  <si>
+    <t>feb/24</t>
+  </si>
+  <si>
+    <t>apr/24</t>
+  </si>
+  <si>
+    <t>may/24</t>
+  </si>
+  <si>
+    <t>aug/24</t>
+  </si>
+  <si>
+    <t>sep/24</t>
   </si>
 </sst>
 </file>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:A22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1373,9 +1373,6 @@
       <c r="M22">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1388,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C8BAD7-93A4-4488-8240-EF1411275326}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2298,6 +2295,9 @@
         <v>0.35</v>
       </c>
     </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>